<commit_message>
Atualização 06/07 - Atualização do construtor da classe TimeSheetManager, com a funcionalidade de verificação e criação da planilha.
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -6,13 +6,29 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Time sheet register" r:id="rId3" sheetId="1"/>
+    <sheet name="PontoEletrônico.xlsx" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>ENTRADA</t>
+  </si>
+  <si>
+    <t>INTERVALO</t>
+  </si>
+  <si>
+    <t>RETORNO INTERVALO</t>
+  </si>
+  <si>
+    <t>SAÍDA</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -55,12 +71,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="6.0859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="9.88671875" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="11.48046875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="21.1484375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="6.66796875" customWidth="true" bestFit="true"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Atualização 08/07 - Importação de batidas de ponto para a planilha está funcional
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -32,16 +32,16 @@
     <t>08/07/2023</t>
   </si>
   <si>
-    <t>12:12:17</t>
+    <t>12:14:59</t>
   </si>
   <si>
-    <t>12:12:18</t>
+    <t>12:15:00</t>
   </si>
   <si>
-    <t>12:12:19</t>
+    <t>12:15:01</t>
   </si>
   <si>
-    <t>12:12:20</t>
+    <t>12:15:02</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Atualização 08/07 - Correção de bug: Uma nova planilha era criada sempre que o programa era aberto novamente.
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>DATA</t>
   </si>
@@ -32,16 +32,40 @@
     <t>08/07/2023</t>
   </si>
   <si>
-    <t>12:14:59</t>
+    <t>12:31:21</t>
   </si>
   <si>
-    <t>12:15:00</t>
+    <t>12:31:22</t>
   </si>
   <si>
-    <t>12:15:01</t>
+    <t>12:31:23</t>
   </si>
   <si>
-    <t>12:15:02</t>
+    <t>12:31:24</t>
+  </si>
+  <si>
+    <t>12:31:43</t>
+  </si>
+  <si>
+    <t>12:31:44</t>
+  </si>
+  <si>
+    <t>12:31:45</t>
+  </si>
+  <si>
+    <t>12:31:46</t>
+  </si>
+  <si>
+    <t>12:32:03</t>
+  </si>
+  <si>
+    <t>12:32:04</t>
+  </si>
+  <si>
+    <t>12:32:05</t>
+  </si>
+  <si>
+    <t>12:32:06</t>
   </si>
 </sst>
 </file>
@@ -86,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -133,6 +157,40 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 09/07 - Programa agora verifica se a bátida atual ja foi realizada no mesmo dia e somente atualiza ela.
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>DATA</t>
   </si>
@@ -29,43 +29,46 @@
     <t>SAÍDA</t>
   </si>
   <si>
-    <t>08/07/2023</t>
+    <t>09/07/2023</t>
   </si>
   <si>
-    <t>12:31:21</t>
+    <t>13:31:21</t>
   </si>
   <si>
-    <t>12:31:22</t>
+    <t>13:31:22</t>
   </si>
   <si>
-    <t>12:31:23</t>
+    <t>13:31:23</t>
   </si>
   <si>
-    <t>12:31:24</t>
+    <t>13:31:24</t>
   </si>
   <si>
-    <t>12:31:43</t>
+    <t>13:32:46</t>
   </si>
   <si>
-    <t>12:31:44</t>
+    <t>13:32:48</t>
   </si>
   <si>
-    <t>12:31:45</t>
+    <t>13:32:49</t>
   </si>
   <si>
-    <t>12:31:46</t>
+    <t>13:32:50</t>
   </si>
   <si>
-    <t>12:32:03</t>
+    <t>10/07/2023</t>
   </si>
   <si>
-    <t>12:32:04</t>
+    <t>13:35:44</t>
   </si>
   <si>
-    <t>12:32:05</t>
+    <t>13:35:45</t>
   </si>
   <si>
-    <t>12:32:06</t>
+    <t>13:35:46</t>
+  </si>
+  <si>
+    <t>13:35:47</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -145,50 +148,33 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização 10/07 - Correção de variáveis, limpando imports inúteis, etc...
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>DATA</t>
   </si>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>13:35:47</t>
+  </si>
+  <si>
+    <t>15:34:29</t>
+  </si>
+  <si>
+    <t>15:34:30</t>
+  </si>
+  <si>
+    <t>15:34:31</t>
+  </si>
+  <si>
+    <t>15:34:33</t>
   </si>
 </sst>
 </file>
@@ -113,7 +125,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -177,6 +189,23 @@
         <v>18</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Atualização 15/07 - Sistema de alteração de batida de ponto finalizado (Todas as funcionalidades básicas do sistema foram implementadas.)
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -37,73 +37,46 @@
     <t xml:space="preserve">SAÍDA</t>
   </si>
   <si>
-    <t xml:space="preserve">09/07/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:32:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:32:48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:32:49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:32:50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10/07/2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:35:44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:35:45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:35:46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13:35:47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:34:29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:34:30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:34:31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15:34:33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:42:05</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:42:06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:42:07</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17:42:08</t>
-  </si>
-  <si>
-    <t>11/07/2023</t>
-  </si>
-  <si>
-    <t>17:43:12</t>
-  </si>
-  <si>
-    <t>17:43:13</t>
-  </si>
-  <si>
-    <t>17:43:14</t>
-  </si>
-  <si>
-    <t>17:43:15</t>
+    <t xml:space="preserve">14/07/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:38:25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:38:26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:38:27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:38:28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15/07/2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:39:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:39:18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:39:19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:39:20</t>
+  </si>
+  <si>
+    <t>07:00:00</t>
+  </si>
+  <si>
+    <t>12:00:00</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
   </si>
 </sst>
 </file>
@@ -203,15 +176,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="7.67" collapsed="false" outlineLevel="0"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="19.58" collapsed="false" outlineLevel="0"/>
     <col min="2" max="2" customWidth="true" hidden="false" style="0" width="12.45" collapsed="false" outlineLevel="0"/>
     <col min="3" max="3" customWidth="true" hidden="false" style="0" width="14.47" collapsed="false" outlineLevel="0"/>
     <col min="4" max="4" customWidth="true" hidden="false" style="0" width="26.66" collapsed="false" outlineLevel="0"/>
@@ -239,17 +212,17 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
+      <c r="B2" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -267,63 +240,6 @@
       </c>
       <c r="E3" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>26</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização 20/07 - Verificação simples da quantidade de batidas inseridas antes de importar os dados para o excel
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>DATA</t>
   </si>
@@ -39,6 +39,30 @@
   </si>
   <si>
     <t>12:31:38</t>
+  </si>
+  <si>
+    <t>20/07/2023</t>
+  </si>
+  <si>
+    <t>21:06:28</t>
+  </si>
+  <si>
+    <t>21:06:30</t>
+  </si>
+  <si>
+    <t>21:06:31</t>
+  </si>
+  <si>
+    <t>22:11:37</t>
+  </si>
+  <si>
+    <t>22:11:38</t>
+  </si>
+  <si>
+    <t>22:11:39</t>
+  </si>
+  <si>
+    <t>22:11:40</t>
   </si>
 </sst>
 </file>
@@ -83,17 +107,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="6.0859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="9.88671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="11.48046875" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.1484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="6.66796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.0859375"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.88671875"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.48046875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="21.1484375"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="6.66796875"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -130,6 +154,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>